<commit_message>
can download titile addr number
</commit_message>
<xml_diff>
--- a/tamplate/arxiv.xlsx
+++ b/tamplate/arxiv.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shijonn\Desktop\cop\automation\tamplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90DC23F3-4692-4DD7-9598-7956EAF3EE0A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{432D7349-C3A8-47A8-8594-26095CB5E7EB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,17 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>编号</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>题目</t>
   </si>
   <si>
-    <t>摘要</t>
-  </si>
-  <si>
     <t>网址</t>
   </si>
   <si>
@@ -41,6 +35,10 @@
   </si>
   <si>
     <t>位置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0-编号</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -84,8 +82,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -388,43 +389,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.26953125" customWidth="1"/>
-    <col min="2" max="2" width="30" customWidth="1"/>
-    <col min="3" max="3" width="55.54296875" customWidth="1"/>
-    <col min="4" max="4" width="36.7265625" customWidth="1"/>
-    <col min="6" max="6" width="15.54296875" customWidth="1"/>
-    <col min="7" max="7" width="18.453125" customWidth="1"/>
+    <col min="2" max="2" width="149.54296875" customWidth="1"/>
+    <col min="3" max="3" width="36.7265625" customWidth="1"/>
+    <col min="5" max="5" width="15.54296875" customWidth="1"/>
+    <col min="6" max="6" width="18.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
record location on excel
</commit_message>
<xml_diff>
--- a/tamplate/arxiv.xlsx
+++ b/tamplate/arxiv.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shijonn\Desktop\cop\automation\tamplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{432D7349-C3A8-47A8-8594-26095CB5E7EB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0017E46-7A44-46B0-A577-3027E3884EF2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -391,7 +391,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -399,8 +399,8 @@
   <cols>
     <col min="1" max="1" width="20.26953125" customWidth="1"/>
     <col min="2" max="2" width="149.54296875" customWidth="1"/>
-    <col min="3" max="3" width="36.7265625" customWidth="1"/>
-    <col min="5" max="5" width="15.54296875" customWidth="1"/>
+    <col min="3" max="3" width="36" customWidth="1"/>
+    <col min="5" max="5" width="22.453125" customWidth="1"/>
     <col min="6" max="6" width="18.453125" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>